<commit_message>
Some changes for different plos journasl
</commit_message>
<xml_diff>
--- a/plosdata/src/main/resources/plos_articles_2.xlsx
+++ b/plosdata/src/main/resources/plos_articles_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="200" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="60" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>PLOS articles citation</t>
   </si>
@@ -48,22 +48,25 @@
     <t>Department of Chemistry and Biochemistry</t>
   </si>
   <si>
-    <t>N/F</t>
-  </si>
-  <si>
-    <t>http://www.plosbiology.org/article/fetchObject.action?uri=info%3Adoi%2F10.1371%2Fjournal.pbio.0030013&amp;representation=PDF</t>
-  </si>
-  <si>
-    <t>10.1371/journal.pbio.0030013</t>
-  </si>
-  <si>
     <t>Bruce A Roe</t>
   </si>
   <si>
     <t>Bedell JA, Budiman MA, Nunberg A, Citek RW, Robbins D, et al. (2005) Sorghum Genome Sequencing by Methylation Filtration. PLoS Biol 3(1): e13. doi:10.1371/journal.pbio.0030013</t>
   </si>
   <si>
-    <t>Repetitive</t>
+    <t>Structure and Dynamics of Amyloid-β Segmental Polymorphisms</t>
+  </si>
+  <si>
+    <t>Workalemahu M. Berhanu</t>
+  </si>
+  <si>
+    <t>Chemistry and Biochemistry</t>
+  </si>
+  <si>
+    <t>Berhanu WM, Hansmann UHE (2012) Structure and Dynamics of Amyloid-β Segmental Polymorphisms. PLoS ONE 7(7): e41479. doi:10.1371/journal.pone.0041479</t>
+  </si>
+  <si>
+    <t>Ulrich H. E. Hansmann</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -195,6 +198,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -509,7 +561,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -537,8 +589,17 @@
     <xf numFmtId="15" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="311">
@@ -1181,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1197,7 +1258,7 @@
     <col min="6" max="6" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="18">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="18">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1205,12 +1266,12 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="16" thickBot="1">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="16" thickBot="1">
       <c r="A2" s="2"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="16" thickBot="1">
+    <row r="3" spans="1:6" ht="16" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1228,7 +1289,7 @@
       </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -1242,37 +1303,53 @@
       <c r="E4" s="12">
         <v>38356</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="F4"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="12">
         <v>38356</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="E6" s="15">
+        <v>41114</v>
+      </c>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>